<commit_message>
add designcourse portfolio example
</commit_message>
<xml_diff>
--- a/code.xlsx
+++ b/code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Symfony\Code\MyWEB-Responsive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81B4BAA-955D-40C1-80BA-71C0906584EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58523F7D-80AF-4C0A-859F-724FDA1EA273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t>OhMyWebSite</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>PortfolioWebsite</t>
+  </si>
+  <si>
+    <t>designcourse-gsportfolio</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -537,7 +540,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -555,21 +558,21 @@
         <v>19</v>
       </c>
       <c r="G2" s="3" t="str">
-        <f t="shared" ref="G2:G14" si="0">_xlfn.CONCAT($B2,$A2,$C2,$A2,$D2)</f>
+        <f t="shared" ref="G2:G15" si="0">_xlfn.CONCAT($B2,$A2,$C2,$A2,$D2)</f>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/Jocker/index.html" target="_blank"&gt;Jocker&lt;/a&gt;
+        &lt;a href="src/designcourse-gsportfolio/index.html" target="_blank"&gt;designcourse-gsportfolio&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
             title="</v>
       </c>
       <c r="H2" s="3" t="str">
-        <f t="shared" ref="H2:H14" si="1">_xlfn.CONCAT($A2,$E2,$A2,$F2)</f>
-        <v xml:space="preserve">Jocker"
-            width="460"
-            height="315"
-            src="src/Jocker/index.html"
+        <f t="shared" ref="H2:H15" si="1">_xlfn.CONCAT($A2,$E2,$A2,$F2)</f>
+        <v xml:space="preserve">designcourse-gsportfolio"
+            width="460"
+            height="315"
+            src="src/designcourse-gsportfolio/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -579,17 +582,17 @@
       </v>
       </c>
       <c r="I2" s="7" t="str">
-        <f t="shared" ref="I2:I14" si="2">_xlfn.CONCAT($G2,$H2)</f>
+        <f t="shared" ref="I2:I15" si="2">_xlfn.CONCAT($G2,$H2)</f>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/Jocker/index.html" target="_blank"&gt;Jocker&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="Jocker"
-            width="460"
-            height="315"
-            src="src/Jocker/index.html"
+        &lt;a href="src/designcourse-gsportfolio/index.html" target="_blank"&gt;designcourse-gsportfolio&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="designcourse-gsportfolio"
+            width="460"
+            height="315"
+            src="src/designcourse-gsportfolio/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -601,7 +604,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -622,7 +625,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/MinimalBlogWebsite/index.html" target="_blank"&gt;MinimalBlogWebsite&lt;/a&gt;
+        &lt;a href="src/Jocker/index.html" target="_blank"&gt;Jocker&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -630,10 +633,10 @@
       </c>
       <c r="H3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">MinimalBlogWebsite"
-            width="460"
-            height="315"
-            src="src/MinimalBlogWebsite/index.html"
+        <v xml:space="preserve">Jocker"
+            width="460"
+            height="315"
+            src="src/Jocker/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -646,14 +649,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/MinimalBlogWebsite/index.html" target="_blank"&gt;MinimalBlogWebsite&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="MinimalBlogWebsite"
-            width="460"
-            height="315"
-            src="src/MinimalBlogWebsite/index.html"
+        &lt;a href="src/Jocker/index.html" target="_blank"&gt;Jocker&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="Jocker"
+            width="460"
+            height="315"
+            src="src/Jocker/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -665,7 +668,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -686,7 +689,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/OhMyWebSite/index.html" target="_blank"&gt;OhMyWebSite&lt;/a&gt;
+        &lt;a href="src/MinimalBlogWebsite/index.html" target="_blank"&gt;MinimalBlogWebsite&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -694,10 +697,10 @@
       </c>
       <c r="H4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">OhMyWebSite"
-            width="460"
-            height="315"
-            src="src/OhMyWebSite/index.html"
+        <v xml:space="preserve">MinimalBlogWebsite"
+            width="460"
+            height="315"
+            src="src/MinimalBlogWebsite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -710,14 +713,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/OhMyWebSite/index.html" target="_blank"&gt;OhMyWebSite&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="OhMyWebSite"
-            width="460"
-            height="315"
-            src="src/OhMyWebSite/index.html"
+        &lt;a href="src/MinimalBlogWebsite/index.html" target="_blank"&gt;MinimalBlogWebsite&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="MinimalBlogWebsite"
+            width="460"
+            height="315"
+            src="src/MinimalBlogWebsite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -729,7 +732,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -750,7 +753,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/PortfolioWebsite/index.html" target="_blank"&gt;PortfolioWebsite&lt;/a&gt;
+        &lt;a href="src/OhMyWebSite/index.html" target="_blank"&gt;OhMyWebSite&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -758,10 +761,10 @@
       </c>
       <c r="H5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">PortfolioWebsite"
-            width="460"
-            height="315"
-            src="src/PortfolioWebsite/index.html"
+        <v xml:space="preserve">OhMyWebSite"
+            width="460"
+            height="315"
+            src="src/OhMyWebSite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -774,14 +777,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/PortfolioWebsite/index.html" target="_blank"&gt;PortfolioWebsite&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="PortfolioWebsite"
-            width="460"
-            height="315"
-            src="src/PortfolioWebsite/index.html"
+        &lt;a href="src/OhMyWebSite/index.html" target="_blank"&gt;OhMyWebSite&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="OhMyWebSite"
+            width="460"
+            height="315"
+            src="src/OhMyWebSite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -793,7 +796,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -814,7 +817,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveCardHover/index.html" target="_blank"&gt;ResponsiveCardHover&lt;/a&gt;
+        &lt;a href="src/PortfolioWebsite/index.html" target="_blank"&gt;PortfolioWebsite&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -822,10 +825,10 @@
       </c>
       <c r="H6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveCardHover"
-            width="460"
-            height="315"
-            src="src/ResponsiveCardHover/index.html"
+        <v xml:space="preserve">PortfolioWebsite"
+            width="460"
+            height="315"
+            src="src/PortfolioWebsite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -838,14 +841,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveCardHover/index.html" target="_blank"&gt;ResponsiveCardHover&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveCardHover"
-            width="460"
-            height="315"
-            src="src/ResponsiveCardHover/index.html"
+        &lt;a href="src/PortfolioWebsite/index.html" target="_blank"&gt;PortfolioWebsite&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="PortfolioWebsite"
+            width="460"
+            height="315"
+            src="src/PortfolioWebsite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -857,7 +860,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -878,7 +881,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html" target="_blank"&gt;ResponsiveDesignCSSImageHoverOverlayEffects&lt;/a&gt;
+        &lt;a href="src/ResponsiveCardHover/index.html" target="_blank"&gt;ResponsiveCardHover&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -886,10 +889,10 @@
       </c>
       <c r="H7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveDesignCSSImageHoverOverlayEffects"
-            width="460"
-            height="315"
-            src="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html"
+        <v xml:space="preserve">ResponsiveCardHover"
+            width="460"
+            height="315"
+            src="src/ResponsiveCardHover/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -902,14 +905,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html" target="_blank"&gt;ResponsiveDesignCSSImageHoverOverlayEffects&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveDesignCSSImageHoverOverlayEffects"
-            width="460"
-            height="315"
-            src="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html"
+        &lt;a href="src/ResponsiveCardHover/index.html" target="_blank"&gt;ResponsiveCardHover&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveCardHover"
+            width="460"
+            height="315"
+            src="src/ResponsiveCardHover/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -921,7 +924,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -942,7 +945,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveFooterCSSGrid/index.html" target="_blank"&gt;ResponsiveFooterCSSGrid&lt;/a&gt;
+        &lt;a href="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html" target="_blank"&gt;ResponsiveDesignCSSImageHoverOverlayEffects&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -950,10 +953,10 @@
       </c>
       <c r="H8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveFooterCSSGrid"
-            width="460"
-            height="315"
-            src="src/ResponsiveFooterCSSGrid/index.html"
+        <v xml:space="preserve">ResponsiveDesignCSSImageHoverOverlayEffects"
+            width="460"
+            height="315"
+            src="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -966,14 +969,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveFooterCSSGrid/index.html" target="_blank"&gt;ResponsiveFooterCSSGrid&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveFooterCSSGrid"
-            width="460"
-            height="315"
-            src="src/ResponsiveFooterCSSGrid/index.html"
+        &lt;a href="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html" target="_blank"&gt;ResponsiveDesignCSSImageHoverOverlayEffects&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveDesignCSSImageHoverOverlayEffects"
+            width="460"
+            height="315"
+            src="src/ResponsiveDesignCSSImageHoverOverlayEffects/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -985,7 +988,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1006,7 +1009,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveHeaderUsingCSSFlex/index.html" target="_blank"&gt;ResponsiveHeaderUsingCSSFlex&lt;/a&gt;
+        &lt;a href="src/ResponsiveFooterCSSGrid/index.html" target="_blank"&gt;ResponsiveFooterCSSGrid&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1014,10 +1017,10 @@
       </c>
       <c r="H9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveHeaderUsingCSSFlex"
-            width="460"
-            height="315"
-            src="src/ResponsiveHeaderUsingCSSFlex/index.html"
+        <v xml:space="preserve">ResponsiveFooterCSSGrid"
+            width="460"
+            height="315"
+            src="src/ResponsiveFooterCSSGrid/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1030,14 +1033,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveHeaderUsingCSSFlex/index.html" target="_blank"&gt;ResponsiveHeaderUsingCSSFlex&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveHeaderUsingCSSFlex"
-            width="460"
-            height="315"
-            src="src/ResponsiveHeaderUsingCSSFlex/index.html"
+        &lt;a href="src/ResponsiveFooterCSSGrid/index.html" target="_blank"&gt;ResponsiveFooterCSSGrid&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveFooterCSSGrid"
+            width="460"
+            height="315"
+            src="src/ResponsiveFooterCSSGrid/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1049,7 +1052,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1070,7 +1073,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveLorukiWebsite/index.html" target="_blank"&gt;ResponsiveLorukiWebsite&lt;/a&gt;
+        &lt;a href="src/ResponsiveHeaderUsingCSSFlex/index.html" target="_blank"&gt;ResponsiveHeaderUsingCSSFlex&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1078,10 +1081,10 @@
       </c>
       <c r="H10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveLorukiWebsite"
-            width="460"
-            height="315"
-            src="src/ResponsiveLorukiWebsite/index.html"
+        <v xml:space="preserve">ResponsiveHeaderUsingCSSFlex"
+            width="460"
+            height="315"
+            src="src/ResponsiveHeaderUsingCSSFlex/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1094,14 +1097,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveLorukiWebsite/index.html" target="_blank"&gt;ResponsiveLorukiWebsite&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveLorukiWebsite"
-            width="460"
-            height="315"
-            src="src/ResponsiveLorukiWebsite/index.html"
+        &lt;a href="src/ResponsiveHeaderUsingCSSFlex/index.html" target="_blank"&gt;ResponsiveHeaderUsingCSSFlex&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveHeaderUsingCSSFlex"
+            width="460"
+            height="315"
+            src="src/ResponsiveHeaderUsingCSSFlex/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1113,7 +1116,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1134,7 +1137,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveTestimonialSlider/index.html" target="_blank"&gt;ResponsiveTestimonialSlider&lt;/a&gt;
+        &lt;a href="src/ResponsiveLorukiWebsite/index.html" target="_blank"&gt;ResponsiveLorukiWebsite&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1142,10 +1145,10 @@
       </c>
       <c r="H11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveTestimonialSlider"
-            width="460"
-            height="315"
-            src="src/ResponsiveTestimonialSlider/index.html"
+        <v xml:space="preserve">ResponsiveLorukiWebsite"
+            width="460"
+            height="315"
+            src="src/ResponsiveLorukiWebsite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1158,14 +1161,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveTestimonialSlider/index.html" target="_blank"&gt;ResponsiveTestimonialSlider&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveTestimonialSlider"
-            width="460"
-            height="315"
-            src="src/ResponsiveTestimonialSlider/index.html"
+        &lt;a href="src/ResponsiveLorukiWebsite/index.html" target="_blank"&gt;ResponsiveLorukiWebsite&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveLorukiWebsite"
+            width="460"
+            height="315"
+            src="src/ResponsiveLorukiWebsite/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1177,7 +1180,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -1198,7 +1201,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveWebsite-02/index.html" target="_blank"&gt;ResponsiveWebsite-02&lt;/a&gt;
+        &lt;a href="src/ResponsiveTestimonialSlider/index.html" target="_blank"&gt;ResponsiveTestimonialSlider&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1206,10 +1209,10 @@
       </c>
       <c r="H12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveWebsite-02"
-            width="460"
-            height="315"
-            src="src/ResponsiveWebsite-02/index.html"
+        <v xml:space="preserve">ResponsiveTestimonialSlider"
+            width="460"
+            height="315"
+            src="src/ResponsiveTestimonialSlider/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1222,14 +1225,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveWebsite-02/index.html" target="_blank"&gt;ResponsiveWebsite-02&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveWebsite-02"
-            width="460"
-            height="315"
-            src="src/ResponsiveWebsite-02/index.html"
+        &lt;a href="src/ResponsiveTestimonialSlider/index.html" target="_blank"&gt;ResponsiveTestimonialSlider&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveTestimonialSlider"
+            width="460"
+            height="315"
+            src="src/ResponsiveTestimonialSlider/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1241,7 +1244,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1262,7 +1265,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveWebsite-03VideoSlider/index.html" target="_blank"&gt;ResponsiveWebsite-03VideoSlider&lt;/a&gt;
+        &lt;a href="src/ResponsiveWebsite-02/index.html" target="_blank"&gt;ResponsiveWebsite-02&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1270,10 +1273,10 @@
       </c>
       <c r="H13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ResponsiveWebsite-03VideoSlider"
-            width="460"
-            height="315"
-            src="src/ResponsiveWebsite-03VideoSlider/index.html"
+        <v xml:space="preserve">ResponsiveWebsite-02"
+            width="460"
+            height="315"
+            src="src/ResponsiveWebsite-02/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1286,14 +1289,14 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveWebsite-03VideoSlider/index.html" target="_blank"&gt;ResponsiveWebsite-03VideoSlider&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="ResponsiveWebsite-03VideoSlider"
-            width="460"
-            height="315"
-            src="src/ResponsiveWebsite-03VideoSlider/index.html"
+        &lt;a href="src/ResponsiveWebsite-02/index.html" target="_blank"&gt;ResponsiveWebsite-02&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveWebsite-02"
+            width="460"
+            height="315"
+            src="src/ResponsiveWebsite-02/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1305,7 +1308,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -1326,7 +1329,7 @@
         <f t="shared" si="0"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/ResponsiveWebsiteFood/index.html" target="_blank"&gt;ResponsiveWebsiteFood&lt;/a&gt;
+        &lt;a href="src/ResponsiveWebsite-03VideoSlider/index.html" target="_blank"&gt;ResponsiveWebsite-03VideoSlider&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1334,6 +1337,70 @@
       </c>
       <c r="H14" s="3" t="str">
         <f t="shared" si="1"/>
+        <v xml:space="preserve">ResponsiveWebsite-03VideoSlider"
+            width="460"
+            height="315"
+            src="src/ResponsiveWebsite-03VideoSlider/index.html"
+            frameborder="0"
+            allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
+            allowfullscreen
+          &gt;&lt;/iframe&gt;
+        &lt;/div&gt;
+      &lt;/section&gt;
+      </v>
+      </c>
+      <c r="I14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">&lt;section&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;a href="src/ResponsiveWebsite-03VideoSlider/index.html" target="_blank"&gt;ResponsiveWebsite-03VideoSlider&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="ResponsiveWebsite-03VideoSlider"
+            width="460"
+            height="315"
+            src="src/ResponsiveWebsite-03VideoSlider/index.html"
+            frameborder="0"
+            allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
+            allowfullscreen
+          &gt;&lt;/iframe&gt;
+        &lt;/div&gt;
+      &lt;/section&gt;
+      </v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;section&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;a href="src/ResponsiveWebsiteFood/index.html" target="_blank"&gt;ResponsiveWebsiteFood&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="</v>
+      </c>
+      <c r="H15" s="3" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">ResponsiveWebsiteFood"
             width="460"
             height="315"
@@ -1346,7 +1413,7 @@
       &lt;/section&gt;
       </v>
       </c>
-      <c r="I14" s="7" t="str">
+      <c r="I15" s="7" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;

</xml_diff>